<commit_message>
v0.10: Update beans squares.
</commit_message>
<xml_diff>
--- a/rsc/all_cases.xlsx
+++ b/rsc/all_cases.xlsx
@@ -21,12 +21,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="24">
   <si>
     <t xml:space="preserve">Start</t>
   </si>
   <si>
-    <t xml:space="preserve">Bonus</t>
+    <t xml:space="preserve">B</t>
   </si>
   <si>
     <t xml:space="preserve">TL</t>
@@ -35,6 +35,9 @@
     <t xml:space="preserve">Replay</t>
   </si>
   <si>
+    <t xml:space="preserve">BBO</t>
+  </si>
+  <si>
     <t xml:space="preserve">Finish</t>
   </si>
   <si>
@@ -77,16 +80,16 @@
     <t xml:space="preserve">COBL</t>
   </si>
   <si>
-    <t xml:space="preserve">VBU</t>
-  </si>
-  <si>
-    <t xml:space="preserve">VBR</t>
-  </si>
-  <si>
-    <t xml:space="preserve">VBD</t>
-  </si>
-  <si>
-    <t xml:space="preserve">VBL</t>
+    <t xml:space="preserve">VNU</t>
+  </si>
+  <si>
+    <t xml:space="preserve">VNR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">VND</t>
+  </si>
+  <si>
+    <t xml:space="preserve">VNL</t>
   </si>
   <si>
     <t xml:space="preserve">bg</t>
@@ -340,7 +343,7 @@
   <dimension ref="B2:E8"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E2" activeCellId="0" sqref="E2"/>
+      <selection pane="topLeft" activeCell="E9" activeCellId="0" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="7.9296875" defaultRowHeight="39.55" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -367,69 +370,69 @@
         <v>3</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E4" s="7" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="39.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B5" s="6" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D5" s="8" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E5" s="7" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="39.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B6" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D6" s="9" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E6" s="10" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="39.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B7" s="8" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="39.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B8" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
   </sheetData>
@@ -461,24 +464,24 @@
   <sheetData>
     <row r="2" customFormat="false" ht="39.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B2" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="39.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="4" customFormat="false" ht="39.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C4" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="39.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D5" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="39.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="7" customFormat="false" ht="39.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D7" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="39.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>

</xml_diff>